<commit_message>
new codelist for readiness
</commit_message>
<xml_diff>
--- a/p_parameters/archive_parameters/Variables_ALG_DP_ROC20_July22.xlsx
+++ b/p_parameters/archive_parameters/Variables_ALG_DP_ROC20_July22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25803"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cduransa/Documents/Utrecht/ROC20/WP3/CVM/Concepts/Codes/ROC20_27_July_2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="8_{B4882D0B-1E25-6A41-BC52-F05044D856B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAE6DC8F-CB36-471F-8078-2FB17A57EC88}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{B4882D0B-1E25-6A41-BC52-F05044D856B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C43FD1C-A27B-4B05-AF88-58020D9DBF43}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="1000" windowWidth="27640" windowHeight="15900" firstSheet="1" xr2:uid="{2506CD93-0285-9E44-BBDD-A2C4E77A0341}"/>
+    <workbookView xWindow="580" yWindow="1000" windowWidth="27640" windowHeight="15900" xr2:uid="{2506CD93-0285-9E44-BBDD-A2C4E77A0341}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="178">
   <si>
     <t>Varname</t>
   </si>
@@ -407,9 +407,6 @@
   </si>
   <si>
     <t>DP_COVSICKLE</t>
-  </si>
-  <si>
-    <t>C_MYOPERICARD_AESI</t>
   </si>
   <si>
     <t>DP_COVCARDIOCEREBROVAS</t>
@@ -672,7 +669,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -991,13 +988,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="35.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1108,7 +1105,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -1117,7 +1114,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3092,10 +3089,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D84700-DED7-384E-8400-81ED0D9F0B97}">
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
@@ -3699,7 +3696,7 @@
         <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>122</v>
+        <v>23</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -3728,7 +3725,7 @@
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -3757,7 +3754,7 @@
         <v>19</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -3786,7 +3783,7 @@
         <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -3815,7 +3812,7 @@
         <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -3844,7 +3841,7 @@
         <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -3873,7 +3870,7 @@
         <v>19</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -3902,7 +3899,7 @@
         <v>19</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -3931,7 +3928,7 @@
         <v>19</v>
       </c>
       <c r="D29" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -3960,7 +3957,7 @@
         <v>19</v>
       </c>
       <c r="D30" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -3986,10 +3983,10 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>123</v>
+        <v>36</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -4018,7 +4015,7 @@
         <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>36</v>
+        <v>123</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -4044,10 +4041,10 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D33" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -4076,7 +4073,7 @@
         <v>48</v>
       </c>
       <c r="D34" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -4102,10 +4099,10 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D35" t="s">
-        <v>125</v>
+        <v>51</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -4134,7 +4131,7 @@
         <v>50</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -4163,7 +4160,7 @@
         <v>50</v>
       </c>
       <c r="D37" t="s">
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -4189,10 +4186,10 @@
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D38" t="s">
-        <v>126</v>
+        <v>51</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -4221,7 +4218,7 @@
         <v>52</v>
       </c>
       <c r="D39" t="s">
-        <v>51</v>
+        <v>125</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -4247,10 +4244,10 @@
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D40" t="s">
-        <v>126</v>
+        <v>74</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -4279,7 +4276,7 @@
         <v>67</v>
       </c>
       <c r="D41" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -4308,7 +4305,7 @@
         <v>67</v>
       </c>
       <c r="D42" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -4337,7 +4334,7 @@
         <v>67</v>
       </c>
       <c r="D43" t="s">
-        <v>69</v>
+        <v>126</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -4363,10 +4360,10 @@
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D44" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -4395,7 +4392,7 @@
         <v>88</v>
       </c>
       <c r="D45" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -4421,10 +4418,10 @@
         <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D46" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -4453,7 +4450,7 @@
         <v>92</v>
       </c>
       <c r="D47" t="s">
-        <v>91</v>
+        <v>128</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -4476,13 +4473,13 @@
         <v>117</v>
       </c>
       <c r="B48" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="D48" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -4511,7 +4508,7 @@
         <v>107</v>
       </c>
       <c r="D49" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -4537,10 +4534,10 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D50" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -4569,7 +4566,7 @@
         <v>104</v>
       </c>
       <c r="D51" t="s">
-        <v>103</v>
+        <v>15</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -4598,7 +4595,7 @@
         <v>104</v>
       </c>
       <c r="D52" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -4621,13 +4618,13 @@
         <v>117</v>
       </c>
       <c r="B53" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>104</v>
+        <v>60</v>
       </c>
       <c r="D53" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -4656,7 +4653,7 @@
         <v>60</v>
       </c>
       <c r="D54" t="s">
-        <v>131</v>
+        <v>59</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -4674,7 +4671,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" ht="15.75">
       <c r="A55" t="s">
         <v>117</v>
       </c>
@@ -4682,10 +4679,10 @@
         <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D55" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -4711,10 +4708,10 @@
         <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>56</v>
+        <v>131</v>
       </c>
       <c r="D56" t="s">
-        <v>55</v>
+        <v>124</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -4740,10 +4737,10 @@
         <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D57" t="s">
-        <v>125</v>
+        <v>54</v>
       </c>
       <c r="F57">
         <v>1</v>
@@ -4769,11 +4766,11 @@
         <v>2</v>
       </c>
       <c r="C58" t="s">
+        <v>131</v>
+      </c>
+      <c r="D58" t="s">
         <v>132</v>
       </c>
-      <c r="D58" t="s">
-        <v>54</v>
-      </c>
       <c r="F58">
         <v>1</v>
       </c>
@@ -4791,17 +4788,17 @@
       </c>
     </row>
     <row r="59" spans="1:10" ht="15.75">
-      <c r="A59" t="s">
-        <v>117</v>
-      </c>
-      <c r="B59" t="s">
-        <v>2</v>
-      </c>
-      <c r="C59" t="s">
-        <v>132</v>
-      </c>
-      <c r="D59" t="s">
-        <v>133</v>
+      <c r="A59" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -4830,7 +4827,7 @@
         <v>6</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -4859,7 +4856,7 @@
         <v>6</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -4888,7 +4885,7 @@
         <v>6</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -4917,7 +4914,7 @@
         <v>6</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -4946,7 +4943,7 @@
         <v>6</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -4964,7 +4961,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="15.75">
+    <row r="65" spans="1:10">
       <c r="A65" s="4" t="s">
         <v>117</v>
       </c>
@@ -4975,7 +4972,7 @@
         <v>6</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -4993,7 +4990,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" ht="15.75">
       <c r="A66" s="4" t="s">
         <v>117</v>
       </c>
@@ -5004,7 +5001,7 @@
         <v>6</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -5019,35 +5016,6 @@
         <v>120</v>
       </c>
       <c r="J66" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="15.75">
-      <c r="A67" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F67">
-        <v>1</v>
-      </c>
-      <c r="G67" t="s">
-        <v>118</v>
-      </c>
-      <c r="H67" t="s">
-        <v>120</v>
-      </c>
-      <c r="I67" t="s">
-        <v>120</v>
-      </c>
-      <c r="J67" t="s">
         <v>120</v>
       </c>
     </row>
@@ -5060,7 +5028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB75E9F1-A72B-7F4F-8E60-3A2250FA444B}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -5076,13 +5044,13 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -5097,18 +5065,18 @@
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="s">
         <v>138</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>139</v>
-      </c>
-      <c r="C2" t="s">
-        <v>140</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -5125,13 +5093,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" t="s">
         <v>141</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>142</v>
-      </c>
-      <c r="C3" t="s">
-        <v>143</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -5148,13 +5116,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" t="s">
         <v>144</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>145</v>
-      </c>
-      <c r="C4" t="s">
-        <v>146</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -5171,13 +5139,13 @@
     </row>
     <row r="5" spans="1:8" ht="15.75">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>147</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>148</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -5197,13 +5165,13 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" t="s">
         <v>149</v>
-      </c>
-      <c r="C6" t="s">
-        <v>150</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -5223,13 +5191,13 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" t="s">
         <v>151</v>
-      </c>
-      <c r="C7" t="s">
-        <v>152</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -5249,13 +5217,13 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" t="s">
         <v>153</v>
-      </c>
-      <c r="C8" t="s">
-        <v>154</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -5275,13 +5243,13 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" t="s">
         <v>155</v>
-      </c>
-      <c r="C9" t="s">
-        <v>156</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -5301,13 +5269,13 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" t="s">
         <v>157</v>
-      </c>
-      <c r="C10" t="s">
-        <v>158</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -5327,13 +5295,13 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" t="s">
         <v>159</v>
-      </c>
-      <c r="C11" t="s">
-        <v>160</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -5356,10 +5324,10 @@
         <v>121</v>
       </c>
       <c r="B12" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" t="s">
         <v>161</v>
-      </c>
-      <c r="C12" t="s">
-        <v>162</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -5379,13 +5347,13 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" t="s">
         <v>163</v>
-      </c>
-      <c r="C13" t="s">
-        <v>164</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -5405,13 +5373,13 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" t="s">
         <v>165</v>
-      </c>
-      <c r="C14" t="s">
-        <v>166</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -5431,13 +5399,13 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15" t="s">
         <v>167</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>168</v>
-      </c>
-      <c r="C15" t="s">
-        <v>169</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -5454,13 +5422,13 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" t="s">
         <v>170</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>171</v>
-      </c>
-      <c r="C16" t="s">
-        <v>172</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -5477,13 +5445,13 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" t="s">
         <v>173</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>174</v>
-      </c>
-      <c r="C17" t="s">
-        <v>175</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -5500,13 +5468,13 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" t="s">
         <v>176</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>177</v>
-      </c>
-      <c r="C18" t="s">
-        <v>178</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -5523,13 +5491,13 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C19" t="s">
         <v>163</v>
-      </c>
-      <c r="C19" t="s">
-        <v>164</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>

</xml_diff>